<commit_message>
Update inventory and master location files
</commit_message>
<xml_diff>
--- a/Empty Bin Formula.xlsx
+++ b/Empty Bin Formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jtlogistics1-my.sharepoint.com/personal/carlos_pacheco_jtlogistics_com2/Documents/bin-helper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6632DA-4999-4B5A-9D4E-E5F2A9AFA688}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82F6A0EB-51D7-4EA8-A4EF-762639CDA797}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D197A4DD-B0B2-47B3-8BB1-E710E3564F08}"/>
   </bookViews>
@@ -799,7 +799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13148518-1423-4096-9C63-2A783C4C38CA}">
   <dimension ref="A1:D2189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B2189"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11778,7 +11780,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1500"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Excel files for Bin Helper logic
</commit_message>
<xml_diff>
--- a/Empty Bin Formula.xlsx
+++ b/Empty Bin Formula.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jtlogistics1-my.sharepoint.com/personal/carlos_pacheco_jtlogistics_com2/Documents/bin-helper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="344" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82F6A0EB-51D7-4EA8-A4EF-762639CDA797}"/>
+  <xr:revisionPtr revIDLastSave="379" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9B5402-04F6-402E-9AD9-E40407B3BC47}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D197A4DD-B0B2-47B3-8BB1-E710E3564F08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D197A4DD-B0B2-47B3-8BB1-E710E3564F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Locations" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>TUN11201</t>
   </si>
@@ -375,13 +375,7 @@
     <t>TUN12316</t>
   </si>
   <si>
-    <t>#N/A =Empty</t>
-  </si>
-  <si>
     <t>Empty Locations</t>
-  </si>
-  <si>
-    <t>689 empty</t>
   </si>
   <si>
     <t>Location</t>
@@ -812,10 +806,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1072,9 +1066,7 @@
       <c r="A52">
         <v>11101703</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2016,85 +2008,82 @@
         <v>11203303</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>11203304</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>11203401</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>11203402</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>11203403</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>11203404</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>11203501</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>11203502</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>11203503</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>11203504</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>11203601</v>
       </c>
-      <c r="D250" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>11203602</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>11203603</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>11203604</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>11300101</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>11300102</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>11300103</v>
       </c>
@@ -11780,7 +11769,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix: Exclude partial bins from Empty Bins view and update master file
</commit_message>
<xml_diff>
--- a/Empty Bin Formula.xlsx
+++ b/Empty Bin Formula.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jtlogistics1-my.sharepoint.com/personal/carlos_pacheco_jtlogistics_com2/Documents/bin-helper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E9B5402-04F6-402E-9AD9-E40407B3BC47}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="8_{81D6FE1D-1782-4D9E-BCFB-B918D277B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EFC8B2F-42F7-4C14-84AE-240A71994C57}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D197A4DD-B0B2-47B3-8BB1-E710E3564F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D197A4DD-B0B2-47B3-8BB1-E710E3564F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Locations" sheetId="1" r:id="rId1"/>
@@ -794,7 +794,7 @@
   <dimension ref="A1:D2189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B2189"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11769,7 +11769,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:A1632"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>